<commit_message>
Bug fixes, deleted debug statements, etc.
Working CODE
</commit_message>
<xml_diff>
--- a/Data_Logger_Variables r1b.xlsx
+++ b/Data_Logger_Variables r1b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="-120" windowWidth="26025" windowHeight="12810"/>
+    <workbookView xWindow="2580" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -740,14 +740,14 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="6" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="6" customWidth="1"/>

</xml_diff>